<commit_message>
Sprint 2 burndown update
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint Backlog/Sprint 2 Burndown.xlsx
+++ b/Sprint 2/Sprint Backlog/Sprint 2 Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony\Documents\Uni\Third year\Semtwo\Agile\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0A1EDE-8A78-4282-BEFD-4A949C48286E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B46D5B5-7AB7-4A1E-8B8B-CFA4A3DE8A0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5A356709-CCAB-495E-BB46-11E884C92558}"/>
   </bookViews>
@@ -382,19 +382,19 @@
                   <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1568,7 +1568,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1634,9 +1634,6 @@
       <c r="B3">
         <v>5</v>
       </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1664,11 +1661,11 @@
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="8">
         <v>3</v>
       </c>
       <c r="D6" s="8"/>
-      <c r="E6" s="2">
+      <c r="E6" s="8">
         <v>3</v>
       </c>
     </row>
@@ -1676,11 +1673,11 @@
       <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="8">
         <v>5</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="8"/>
       <c r="F7">
         <v>3</v>
       </c>
@@ -1695,6 +1692,9 @@
       <c r="B8">
         <v>5</v>
       </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1703,7 +1703,18 @@
       <c r="B9">
         <v>5</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8">
+        <v>-1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1750,7 +1761,7 @@
       <c r="B14">
         <v>2</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1773,6 +1784,9 @@
       <c r="B16">
         <v>2</v>
       </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -1791,7 +1805,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B19" s="4"/>
+      <c r="B19" s="8"/>
       <c r="J19" s="5" t="s">
         <v>10</v>
       </c>
@@ -1807,7 +1821,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F20" s="3"/>
+      <c r="F20" s="8"/>
       <c r="K20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1826,7 +1840,7 @@
       </c>
       <c r="D21">
         <f>C21-SUM(D3:D20)</f>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21">
         <f>D21-SUM(E3:E20)</f>
@@ -1834,15 +1848,15 @@
       </c>
       <c r="F21">
         <f>E21-SUM(F3:F20)</f>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G21">
         <f>F21-SUM(G3:G20)</f>
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H21">
         <f>G21-SUM(H3:H20)</f>
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>11</v>

</xml_diff>